<commit_message>
MPG Synthetic Data,.csv format
</commit_message>
<xml_diff>
--- a/MPG_Data/Data_MPG_Original.xlsx
+++ b/MPG_Data/Data_MPG_Original.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="315">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="314">
   <si>
     <t>mpg</t>
   </si>
@@ -131,9 +131,6 @@
   </si>
   <si>
     <t>toyota corona</t>
-  </si>
-  <si>
-    <t>?</t>
   </si>
   <si>
     <t>ford pinto</t>
@@ -1983,9 +1980,7 @@
       <c r="C34" s="1">
         <v>98.0</v>
       </c>
-      <c r="D34" s="1" t="s">
-        <v>40</v>
-      </c>
+      <c r="D34" s="1"/>
       <c r="E34" s="1">
         <v>2046.0</v>
       </c>
@@ -1999,7 +1994,7 @@
         <v>1.0</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="35">
@@ -2057,7 +2052,7 @@
         <v>1.0</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="37">
@@ -2115,7 +2110,7 @@
         <v>1.0</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="39">
@@ -2144,7 +2139,7 @@
         <v>1.0</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="40">
@@ -2202,7 +2197,7 @@
         <v>1.0</v>
       </c>
       <c r="I41" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="42">
@@ -2289,7 +2284,7 @@
         <v>1.0</v>
       </c>
       <c r="I44" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="45">
@@ -2318,7 +2313,7 @@
         <v>1.0</v>
       </c>
       <c r="I45" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="46">
@@ -2347,7 +2342,7 @@
         <v>1.0</v>
       </c>
       <c r="I46" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="47">
@@ -2376,7 +2371,7 @@
         <v>1.0</v>
       </c>
       <c r="I47" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="48">
@@ -2405,7 +2400,7 @@
         <v>1.0</v>
       </c>
       <c r="I48" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="49">
@@ -2434,7 +2429,7 @@
         <v>1.0</v>
       </c>
       <c r="I49" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="50">
@@ -2463,7 +2458,7 @@
         <v>1.0</v>
       </c>
       <c r="I50" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="51">
@@ -2492,7 +2487,7 @@
         <v>1.0</v>
       </c>
       <c r="I51" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="52">
@@ -2521,7 +2516,7 @@
         <v>2.0</v>
       </c>
       <c r="I52" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="53">
@@ -2550,7 +2545,7 @@
         <v>2.0</v>
       </c>
       <c r="I53" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="54">
@@ -2579,7 +2574,7 @@
         <v>2.0</v>
       </c>
       <c r="I54" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="55">
@@ -2608,7 +2603,7 @@
         <v>3.0</v>
       </c>
       <c r="I55" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="56">
@@ -2637,7 +2632,7 @@
         <v>3.0</v>
       </c>
       <c r="I56" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="57">
@@ -2666,7 +2661,7 @@
         <v>2.0</v>
       </c>
       <c r="I57" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="58">
@@ -2695,7 +2690,7 @@
         <v>1.0</v>
       </c>
       <c r="I58" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="59">
@@ -2724,7 +2719,7 @@
         <v>3.0</v>
       </c>
       <c r="I59" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="60">
@@ -2753,7 +2748,7 @@
         <v>1.0</v>
       </c>
       <c r="I60" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="61">
@@ -2782,7 +2777,7 @@
         <v>2.0</v>
       </c>
       <c r="I61" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="62">
@@ -2811,7 +2806,7 @@
         <v>1.0</v>
       </c>
       <c r="I62" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="63">
@@ -2840,7 +2835,7 @@
         <v>1.0</v>
       </c>
       <c r="I63" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="64">
@@ -2985,7 +2980,7 @@
         <v>1.0</v>
       </c>
       <c r="I68" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="69">
@@ -3014,7 +3009,7 @@
         <v>1.0</v>
       </c>
       <c r="I69" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="70">
@@ -3043,7 +3038,7 @@
         <v>1.0</v>
       </c>
       <c r="I70" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="71">
@@ -3072,7 +3067,7 @@
         <v>1.0</v>
       </c>
       <c r="I71" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="72">
@@ -3101,7 +3096,7 @@
         <v>1.0</v>
       </c>
       <c r="I72" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="73">
@@ -3130,7 +3125,7 @@
         <v>3.0</v>
       </c>
       <c r="I73" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="74">
@@ -3159,7 +3154,7 @@
         <v>1.0</v>
       </c>
       <c r="I74" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="75">
@@ -3188,7 +3183,7 @@
         <v>1.0</v>
       </c>
       <c r="I75" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="76">
@@ -3217,7 +3212,7 @@
         <v>1.0</v>
       </c>
       <c r="I76" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="77">
@@ -3246,7 +3241,7 @@
         <v>1.0</v>
       </c>
       <c r="I77" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="78">
@@ -3275,7 +3270,7 @@
         <v>2.0</v>
       </c>
       <c r="I78" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="79">
@@ -3304,7 +3299,7 @@
         <v>2.0</v>
       </c>
       <c r="I79" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="80">
@@ -3333,7 +3328,7 @@
         <v>2.0</v>
       </c>
       <c r="I80" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="81">
@@ -3362,7 +3357,7 @@
         <v>2.0</v>
       </c>
       <c r="I81" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="82">
@@ -3391,7 +3386,7 @@
         <v>1.0</v>
       </c>
       <c r="I82" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="83">
@@ -3420,7 +3415,7 @@
         <v>3.0</v>
       </c>
       <c r="I83" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="84">
@@ -3449,7 +3444,7 @@
         <v>3.0</v>
       </c>
       <c r="I84" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="85">
@@ -3478,7 +3473,7 @@
         <v>1.0</v>
       </c>
       <c r="I85" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="86">
@@ -3507,7 +3502,7 @@
         <v>3.0</v>
       </c>
       <c r="I86" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="87">
@@ -3536,7 +3531,7 @@
         <v>1.0</v>
       </c>
       <c r="I87" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="88">
@@ -3565,7 +3560,7 @@
         <v>1.0</v>
       </c>
       <c r="I88" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="89">
@@ -3594,7 +3589,7 @@
         <v>1.0</v>
       </c>
       <c r="I89" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="90">
@@ -3623,7 +3618,7 @@
         <v>1.0</v>
       </c>
       <c r="I90" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="91">
@@ -3652,7 +3647,7 @@
         <v>1.0</v>
       </c>
       <c r="I91" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="92">
@@ -3681,7 +3676,7 @@
         <v>1.0</v>
       </c>
       <c r="I92" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="93">
@@ -3710,7 +3705,7 @@
         <v>1.0</v>
       </c>
       <c r="I93" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="94">
@@ -3739,7 +3734,7 @@
         <v>1.0</v>
       </c>
       <c r="I94" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="95">
@@ -3768,7 +3763,7 @@
         <v>1.0</v>
       </c>
       <c r="I95" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="96">
@@ -3797,7 +3792,7 @@
         <v>1.0</v>
       </c>
       <c r="I96" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="97">
@@ -3826,7 +3821,7 @@
         <v>1.0</v>
       </c>
       <c r="I97" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="98">
@@ -3855,7 +3850,7 @@
         <v>1.0</v>
       </c>
       <c r="I98" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="99">
@@ -3884,7 +3879,7 @@
         <v>1.0</v>
       </c>
       <c r="I99" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="100">
@@ -3913,7 +3908,7 @@
         <v>1.0</v>
       </c>
       <c r="I100" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="101">
@@ -4029,7 +4024,7 @@
         <v>2.0</v>
       </c>
       <c r="I104" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="105">
@@ -4087,7 +4082,7 @@
         <v>1.0</v>
       </c>
       <c r="I106" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="107">
@@ -4116,7 +4111,7 @@
         <v>1.0</v>
       </c>
       <c r="I107" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="108">
@@ -4145,7 +4140,7 @@
         <v>1.0</v>
       </c>
       <c r="I108" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="109">
@@ -4203,7 +4198,7 @@
         <v>3.0</v>
       </c>
       <c r="I110" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="111">
@@ -4232,7 +4227,7 @@
         <v>1.0</v>
       </c>
       <c r="I111" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="112">
@@ -4261,7 +4256,7 @@
         <v>3.0</v>
       </c>
       <c r="I112" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="113">
@@ -4290,7 +4285,7 @@
         <v>3.0</v>
       </c>
       <c r="I113" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="114">
@@ -4319,7 +4314,7 @@
         <v>1.0</v>
       </c>
       <c r="I114" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="115">
@@ -4348,7 +4343,7 @@
         <v>1.0</v>
       </c>
       <c r="I115" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="116">
@@ -4377,7 +4372,7 @@
         <v>2.0</v>
       </c>
       <c r="I116" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="117">
@@ -4406,7 +4401,7 @@
         <v>1.0</v>
       </c>
       <c r="I117" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="118">
@@ -4435,7 +4430,7 @@
         <v>1.0</v>
       </c>
       <c r="I118" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="119">
@@ -4464,7 +4459,7 @@
         <v>2.0</v>
       </c>
       <c r="I119" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="120">
@@ -4493,7 +4488,7 @@
         <v>2.0</v>
       </c>
       <c r="I120" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="121">
@@ -4522,7 +4517,7 @@
         <v>2.0</v>
       </c>
       <c r="I121" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="122">
@@ -4551,7 +4546,7 @@
         <v>2.0</v>
       </c>
       <c r="I122" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="123">
@@ -4580,7 +4575,7 @@
         <v>1.0</v>
       </c>
       <c r="I123" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="124">
@@ -4609,7 +4604,7 @@
         <v>2.0</v>
       </c>
       <c r="I124" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="125">
@@ -4638,7 +4633,7 @@
         <v>3.0</v>
       </c>
       <c r="I125" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="126">
@@ -4667,7 +4662,7 @@
         <v>1.0</v>
       </c>
       <c r="I126" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="127">
@@ -4709,9 +4704,7 @@
       <c r="C128" s="1">
         <v>200.0</v>
       </c>
-      <c r="D128" s="1" t="s">
-        <v>40</v>
-      </c>
+      <c r="D128" s="1"/>
       <c r="E128" s="1">
         <v>2875.0</v>
       </c>
@@ -4783,7 +4776,7 @@
         <v>1.0</v>
       </c>
       <c r="I130" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="131">
@@ -4812,7 +4805,7 @@
         <v>3.0</v>
       </c>
       <c r="I131" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="132">
@@ -4841,7 +4834,7 @@
         <v>1.0</v>
       </c>
       <c r="I132" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="133">
@@ -4870,7 +4863,7 @@
         <v>3.0</v>
       </c>
       <c r="I133" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="134">
@@ -4899,7 +4892,7 @@
         <v>1.0</v>
       </c>
       <c r="I134" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="135">
@@ -4928,7 +4921,7 @@
         <v>1.0</v>
       </c>
       <c r="I135" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="136">
@@ -4957,7 +4950,7 @@
         <v>1.0</v>
       </c>
       <c r="I136" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="137">
@@ -4986,7 +4979,7 @@
         <v>1.0</v>
       </c>
       <c r="I137" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="138">
@@ -5015,7 +5008,7 @@
         <v>1.0</v>
       </c>
       <c r="I138" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="139">
@@ -5044,7 +5037,7 @@
         <v>1.0</v>
       </c>
       <c r="I139" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="140">
@@ -5073,7 +5066,7 @@
         <v>1.0</v>
       </c>
       <c r="I140" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="141">
@@ -5102,7 +5095,7 @@
         <v>1.0</v>
       </c>
       <c r="I141" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="142">
@@ -5131,7 +5124,7 @@
         <v>1.0</v>
       </c>
       <c r="I142" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="143">
@@ -5160,7 +5153,7 @@
         <v>2.0</v>
       </c>
       <c r="I143" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="144">
@@ -5189,7 +5182,7 @@
         <v>2.0</v>
       </c>
       <c r="I144" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="145">
@@ -5218,7 +5211,7 @@
         <v>2.0</v>
       </c>
       <c r="I145" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="146">
@@ -5276,7 +5269,7 @@
         <v>3.0</v>
       </c>
       <c r="I147" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="148">
@@ -5305,7 +5298,7 @@
         <v>1.0</v>
       </c>
       <c r="I148" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="149">
@@ -5334,7 +5327,7 @@
         <v>2.0</v>
       </c>
       <c r="I149" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="150">
@@ -5363,7 +5356,7 @@
         <v>2.0</v>
       </c>
       <c r="I150" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="151">
@@ -5392,7 +5385,7 @@
         <v>3.0</v>
       </c>
       <c r="I151" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="152">
@@ -5421,7 +5414,7 @@
         <v>3.0</v>
       </c>
       <c r="I152" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="153">
@@ -5450,7 +5443,7 @@
         <v>2.0</v>
       </c>
       <c r="I153" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="154">
@@ -5479,7 +5472,7 @@
         <v>1.0</v>
       </c>
       <c r="I154" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="155">
@@ -5508,7 +5501,7 @@
         <v>1.0</v>
       </c>
       <c r="I155" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="156">
@@ -5537,7 +5530,7 @@
         <v>1.0</v>
       </c>
       <c r="I156" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="157">
@@ -5624,7 +5617,7 @@
         <v>1.0</v>
       </c>
       <c r="I159" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="160">
@@ -5653,7 +5646,7 @@
         <v>1.0</v>
       </c>
       <c r="I160" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="161">
@@ -5682,7 +5675,7 @@
         <v>1.0</v>
       </c>
       <c r="I161" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="162">
@@ -5711,7 +5704,7 @@
         <v>1.0</v>
       </c>
       <c r="I162" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="163">
@@ -5740,7 +5733,7 @@
         <v>1.0</v>
       </c>
       <c r="I163" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="164">
@@ -5769,7 +5762,7 @@
         <v>1.0</v>
       </c>
       <c r="I164" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="165">
@@ -5798,7 +5791,7 @@
         <v>1.0</v>
       </c>
       <c r="I165" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="166">
@@ -5827,7 +5820,7 @@
         <v>1.0</v>
       </c>
       <c r="I166" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="167">
@@ -5856,7 +5849,7 @@
         <v>1.0</v>
       </c>
       <c r="I167" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="168">
@@ -5885,7 +5878,7 @@
         <v>1.0</v>
       </c>
       <c r="I168" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="169">
@@ -5914,7 +5907,7 @@
         <v>3.0</v>
       </c>
       <c r="I169" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="170">
@@ -5943,7 +5936,7 @@
         <v>1.0</v>
       </c>
       <c r="I170" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="171">
@@ -6001,7 +5994,7 @@
         <v>1.0</v>
       </c>
       <c r="I172" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="173">
@@ -6059,7 +6052,7 @@
         <v>2.0</v>
       </c>
       <c r="I174" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="175">
@@ -6088,7 +6081,7 @@
         <v>3.0</v>
       </c>
       <c r="I175" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="176">
@@ -6117,7 +6110,7 @@
         <v>1.0</v>
       </c>
       <c r="I176" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="177">
@@ -6146,7 +6139,7 @@
         <v>2.0</v>
       </c>
       <c r="I177" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="178">
@@ -6175,7 +6168,7 @@
         <v>1.0</v>
       </c>
       <c r="I178" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="179">
@@ -6204,7 +6197,7 @@
         <v>2.0</v>
       </c>
       <c r="I179" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="180">
@@ -6262,7 +6255,7 @@
         <v>2.0</v>
       </c>
       <c r="I181" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="182">
@@ -6291,7 +6284,7 @@
         <v>2.0</v>
       </c>
       <c r="I182" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="183">
@@ -6320,7 +6313,7 @@
         <v>3.0</v>
       </c>
       <c r="I183" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="184">
@@ -6349,7 +6342,7 @@
         <v>2.0</v>
       </c>
       <c r="I184" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="185">
@@ -6378,7 +6371,7 @@
         <v>2.0</v>
       </c>
       <c r="I185" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="186">
@@ -6407,7 +6400,7 @@
         <v>1.0</v>
       </c>
       <c r="I186" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="187">
@@ -6436,7 +6429,7 @@
         <v>1.0</v>
       </c>
       <c r="I187" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="188">
@@ -6465,7 +6458,7 @@
         <v>2.0</v>
       </c>
       <c r="I188" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="189">
@@ -6494,7 +6487,7 @@
         <v>1.0</v>
       </c>
       <c r="I189" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="190">
@@ -6523,7 +6516,7 @@
         <v>1.0</v>
       </c>
       <c r="I190" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="191">
@@ -6552,7 +6545,7 @@
         <v>1.0</v>
       </c>
       <c r="I191" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="192">
@@ -6581,7 +6574,7 @@
         <v>1.0</v>
       </c>
       <c r="I192" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="193">
@@ -6610,7 +6603,7 @@
         <v>1.0</v>
       </c>
       <c r="I193" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="194">
@@ -6639,7 +6632,7 @@
         <v>1.0</v>
       </c>
       <c r="I194" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="195">
@@ -6726,7 +6719,7 @@
         <v>1.0</v>
       </c>
       <c r="I197" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="198">
@@ -6755,7 +6748,7 @@
         <v>1.0</v>
       </c>
       <c r="I198" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="199">
@@ -6784,7 +6777,7 @@
         <v>2.0</v>
       </c>
       <c r="I199" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="200">
@@ -6813,7 +6806,7 @@
         <v>3.0</v>
       </c>
       <c r="I200" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="201">
@@ -6842,7 +6835,7 @@
         <v>1.0</v>
       </c>
       <c r="I201" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="202">
@@ -6871,7 +6864,7 @@
         <v>1.0</v>
       </c>
       <c r="I202" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="203">
@@ -6900,7 +6893,7 @@
         <v>1.0</v>
       </c>
       <c r="I203" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="204">
@@ -6929,7 +6922,7 @@
         <v>1.0</v>
       </c>
       <c r="I204" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="205">
@@ -6958,7 +6951,7 @@
         <v>2.0</v>
       </c>
       <c r="I205" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="206">
@@ -6987,7 +6980,7 @@
         <v>3.0</v>
       </c>
       <c r="I206" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="207">
@@ -7016,7 +7009,7 @@
         <v>3.0</v>
       </c>
       <c r="I207" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="208">
@@ -7045,7 +7038,7 @@
         <v>1.0</v>
       </c>
       <c r="I208" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="209">
@@ -7074,7 +7067,7 @@
         <v>2.0</v>
       </c>
       <c r="I209" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="210">
@@ -7103,7 +7096,7 @@
         <v>1.0</v>
       </c>
       <c r="I210" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="211">
@@ -7161,7 +7154,7 @@
         <v>3.0</v>
       </c>
       <c r="I212" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="213">
@@ -7190,7 +7183,7 @@
         <v>2.0</v>
       </c>
       <c r="I213" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="214">
@@ -7219,7 +7212,7 @@
         <v>1.0</v>
       </c>
       <c r="I214" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="215">
@@ -7248,7 +7241,7 @@
         <v>1.0</v>
       </c>
       <c r="I215" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="216">
@@ -7277,7 +7270,7 @@
         <v>1.0</v>
       </c>
       <c r="I216" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="217">
@@ -7306,7 +7299,7 @@
         <v>1.0</v>
       </c>
       <c r="I217" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="218">
@@ -7335,7 +7328,7 @@
         <v>3.0</v>
       </c>
       <c r="I218" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="219">
@@ -7364,7 +7357,7 @@
         <v>1.0</v>
       </c>
       <c r="I219" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="220">
@@ -7393,7 +7386,7 @@
         <v>2.0</v>
       </c>
       <c r="I220" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="221">
@@ -7422,7 +7415,7 @@
         <v>1.0</v>
       </c>
       <c r="I221" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="222">
@@ -7451,7 +7444,7 @@
         <v>3.0</v>
       </c>
       <c r="I222" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="223">
@@ -7480,7 +7473,7 @@
         <v>1.0</v>
       </c>
       <c r="I223" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="224">
@@ -7509,7 +7502,7 @@
         <v>1.0</v>
       </c>
       <c r="I224" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="225">
@@ -7538,7 +7531,7 @@
         <v>1.0</v>
       </c>
       <c r="I225" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="226">
@@ -7567,7 +7560,7 @@
         <v>1.0</v>
       </c>
       <c r="I226" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="227">
@@ -7596,7 +7589,7 @@
         <v>1.0</v>
       </c>
       <c r="I227" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="228">
@@ -7625,7 +7618,7 @@
         <v>1.0</v>
       </c>
       <c r="I228" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="229">
@@ -7654,7 +7647,7 @@
         <v>1.0</v>
       </c>
       <c r="I229" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="230">
@@ -7683,7 +7676,7 @@
         <v>1.0</v>
       </c>
       <c r="I230" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="231">
@@ -7712,7 +7705,7 @@
         <v>1.0</v>
       </c>
       <c r="I231" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="232">
@@ -7741,7 +7734,7 @@
         <v>1.0</v>
       </c>
       <c r="I232" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="233">
@@ -7770,7 +7763,7 @@
         <v>1.0</v>
       </c>
       <c r="I233" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="234">
@@ -7799,7 +7792,7 @@
         <v>1.0</v>
       </c>
       <c r="I234" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="235">
@@ -7828,7 +7821,7 @@
         <v>2.0</v>
       </c>
       <c r="I235" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="236">
@@ -7857,7 +7850,7 @@
         <v>1.0</v>
       </c>
       <c r="I236" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="237">
@@ -7886,7 +7879,7 @@
         <v>3.0</v>
       </c>
       <c r="I237" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="238">
@@ -7915,7 +7908,7 @@
         <v>1.0</v>
       </c>
       <c r="I238" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="239">
@@ -7944,7 +7937,7 @@
         <v>1.0</v>
       </c>
       <c r="I239" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="240">
@@ -7973,7 +7966,7 @@
         <v>1.0</v>
       </c>
       <c r="I240" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="241">
@@ -8002,7 +7995,7 @@
         <v>3.0</v>
       </c>
       <c r="I241" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="242">
@@ -8031,7 +8024,7 @@
         <v>2.0</v>
       </c>
       <c r="I242" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="243">
@@ -8060,7 +8053,7 @@
         <v>3.0</v>
       </c>
       <c r="I243" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="244">
@@ -8089,7 +8082,7 @@
         <v>2.0</v>
       </c>
       <c r="I244" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="245">
@@ -8118,7 +8111,7 @@
         <v>3.0</v>
       </c>
       <c r="I245" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="246">
@@ -8147,7 +8140,7 @@
         <v>2.0</v>
       </c>
       <c r="I246" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="247">
@@ -8176,7 +8169,7 @@
         <v>1.0</v>
       </c>
       <c r="I247" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="248">
@@ -8205,7 +8198,7 @@
         <v>3.0</v>
       </c>
       <c r="I248" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="249">
@@ -8234,7 +8227,7 @@
         <v>3.0</v>
       </c>
       <c r="I249" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="250">
@@ -8263,7 +8256,7 @@
         <v>3.0</v>
       </c>
       <c r="I250" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="251">
@@ -8292,7 +8285,7 @@
         <v>1.0</v>
       </c>
       <c r="I251" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="252">
@@ -8321,7 +8314,7 @@
         <v>1.0</v>
       </c>
       <c r="I252" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="253">
@@ -8350,7 +8343,7 @@
         <v>1.0</v>
       </c>
       <c r="I253" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="254">
@@ -8379,7 +8372,7 @@
         <v>1.0</v>
       </c>
       <c r="I254" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="255">
@@ -8408,7 +8401,7 @@
         <v>1.0</v>
       </c>
       <c r="I255" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="256">
@@ -8437,7 +8430,7 @@
         <v>1.0</v>
       </c>
       <c r="I256" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="257">
@@ -8466,7 +8459,7 @@
         <v>1.0</v>
       </c>
       <c r="I257" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="258">
@@ -8495,7 +8488,7 @@
         <v>1.0</v>
       </c>
       <c r="I258" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="259">
@@ -8524,7 +8517,7 @@
         <v>1.0</v>
       </c>
       <c r="I259" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="260">
@@ -8553,7 +8546,7 @@
         <v>1.0</v>
       </c>
       <c r="I260" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="261">
@@ -8582,7 +8575,7 @@
         <v>1.0</v>
       </c>
       <c r="I261" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="262">
@@ -8611,7 +8604,7 @@
         <v>1.0</v>
       </c>
       <c r="I262" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="263">
@@ -8640,7 +8633,7 @@
         <v>1.0</v>
       </c>
       <c r="I263" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="264">
@@ -8669,7 +8662,7 @@
         <v>1.0</v>
       </c>
       <c r="I264" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="265">
@@ -8698,7 +8691,7 @@
         <v>1.0</v>
       </c>
       <c r="I265" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="266">
@@ -8727,7 +8720,7 @@
         <v>1.0</v>
       </c>
       <c r="I266" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="267">
@@ -8756,7 +8749,7 @@
         <v>1.0</v>
       </c>
       <c r="I267" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="268">
@@ -8785,7 +8778,7 @@
         <v>1.0</v>
       </c>
       <c r="I268" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="269">
@@ -8843,7 +8836,7 @@
         <v>3.0</v>
       </c>
       <c r="I270" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="271">
@@ -8872,7 +8865,7 @@
         <v>1.0</v>
       </c>
       <c r="I271" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="272">
@@ -8901,7 +8894,7 @@
         <v>3.0</v>
       </c>
       <c r="I272" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="273">
@@ -8930,7 +8923,7 @@
         <v>1.0</v>
       </c>
       <c r="I273" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="274">
@@ -8959,7 +8952,7 @@
         <v>1.0</v>
       </c>
       <c r="I274" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="275">
@@ -8988,7 +8981,7 @@
         <v>3.0</v>
       </c>
       <c r="I275" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="276">
@@ -9017,7 +9010,7 @@
         <v>2.0</v>
       </c>
       <c r="I276" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="277">
@@ -9046,7 +9039,7 @@
         <v>2.0</v>
       </c>
       <c r="I277" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="278">
@@ -9075,7 +9068,7 @@
         <v>2.0</v>
       </c>
       <c r="I278" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="279">
@@ -9104,7 +9097,7 @@
         <v>2.0</v>
       </c>
       <c r="I279" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="280">
@@ -9133,7 +9126,7 @@
         <v>2.0</v>
       </c>
       <c r="I280" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="281">
@@ -9162,7 +9155,7 @@
         <v>3.0</v>
       </c>
       <c r="I281" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="282">
@@ -9191,7 +9184,7 @@
         <v>1.0</v>
       </c>
       <c r="I282" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="283">
@@ -9220,7 +9213,7 @@
         <v>1.0</v>
       </c>
       <c r="I283" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="284">
@@ -9249,7 +9242,7 @@
         <v>1.0</v>
       </c>
       <c r="I284" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="285">
@@ -9278,7 +9271,7 @@
         <v>1.0</v>
       </c>
       <c r="I285" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="286">
@@ -9307,7 +9300,7 @@
         <v>1.0</v>
       </c>
       <c r="I286" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="287">
@@ -9336,7 +9329,7 @@
         <v>1.0</v>
       </c>
       <c r="I287" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="288">
@@ -9365,7 +9358,7 @@
         <v>1.0</v>
       </c>
       <c r="I288" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="289">
@@ -9394,7 +9387,7 @@
         <v>1.0</v>
       </c>
       <c r="I289" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="290">
@@ -9423,7 +9416,7 @@
         <v>1.0</v>
       </c>
       <c r="I290" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="291">
@@ -9481,7 +9474,7 @@
         <v>1.0</v>
       </c>
       <c r="I292" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="293">
@@ -9510,7 +9503,7 @@
         <v>1.0</v>
       </c>
       <c r="I293" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="294">
@@ -9539,7 +9532,7 @@
         <v>1.0</v>
       </c>
       <c r="I294" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="295">
@@ -9568,7 +9561,7 @@
         <v>2.0</v>
       </c>
       <c r="I295" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="296">
@@ -9597,7 +9590,7 @@
         <v>3.0</v>
       </c>
       <c r="I296" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="297">
@@ -9626,7 +9619,7 @@
         <v>1.0</v>
       </c>
       <c r="I297" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="298">
@@ -9655,7 +9648,7 @@
         <v>1.0</v>
       </c>
       <c r="I298" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="299">
@@ -9684,7 +9677,7 @@
         <v>2.0</v>
       </c>
       <c r="I299" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="300">
@@ -9713,7 +9706,7 @@
         <v>1.0</v>
       </c>
       <c r="I300" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="301">
@@ -9771,7 +9764,7 @@
         <v>1.0</v>
       </c>
       <c r="I302" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="303">
@@ -9800,7 +9793,7 @@
         <v>1.0</v>
       </c>
       <c r="I303" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="304">
@@ -9829,7 +9822,7 @@
         <v>1.0</v>
       </c>
       <c r="I304" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="305">
@@ -9858,7 +9851,7 @@
         <v>3.0</v>
       </c>
       <c r="I305" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="306">
@@ -9887,7 +9880,7 @@
         <v>2.0</v>
       </c>
       <c r="I306" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="307">
@@ -9916,7 +9909,7 @@
         <v>1.0</v>
       </c>
       <c r="I307" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="308">
@@ -9945,7 +9938,7 @@
         <v>1.0</v>
       </c>
       <c r="I308" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="309">
@@ -9974,7 +9967,7 @@
         <v>1.0</v>
       </c>
       <c r="I309" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="310">
@@ -10003,7 +9996,7 @@
         <v>1.0</v>
       </c>
       <c r="I310" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="311">
@@ -10032,7 +10025,7 @@
         <v>2.0</v>
       </c>
       <c r="I311" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="312">
@@ -10061,7 +10054,7 @@
         <v>3.0</v>
       </c>
       <c r="I312" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="313">
@@ -10090,7 +10083,7 @@
         <v>1.0</v>
       </c>
       <c r="I313" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="314">
@@ -10119,7 +10112,7 @@
         <v>3.0</v>
       </c>
       <c r="I314" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="315">
@@ -10148,7 +10141,7 @@
         <v>1.0</v>
       </c>
       <c r="I315" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="316">
@@ -10177,7 +10170,7 @@
         <v>1.0</v>
       </c>
       <c r="I316" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="317">
@@ -10206,7 +10199,7 @@
         <v>1.0</v>
       </c>
       <c r="I317" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="318">
@@ -10235,7 +10228,7 @@
         <v>1.0</v>
       </c>
       <c r="I318" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="319">
@@ -10264,7 +10257,7 @@
         <v>2.0</v>
       </c>
       <c r="I319" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="320">
@@ -10293,7 +10286,7 @@
         <v>3.0</v>
       </c>
       <c r="I320" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="321">
@@ -10322,7 +10315,7 @@
         <v>3.0</v>
       </c>
       <c r="I321" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="322">
@@ -10351,7 +10344,7 @@
         <v>3.0</v>
       </c>
       <c r="I322" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="323">
@@ -10380,7 +10373,7 @@
         <v>3.0</v>
       </c>
       <c r="I323" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="324">
@@ -10409,7 +10402,7 @@
         <v>3.0</v>
       </c>
       <c r="I324" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="325">
@@ -10438,7 +10431,7 @@
         <v>1.0</v>
       </c>
       <c r="I325" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="326">
@@ -10467,7 +10460,7 @@
         <v>3.0</v>
       </c>
       <c r="I326" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="327">
@@ -10496,7 +10489,7 @@
         <v>2.0</v>
       </c>
       <c r="I327" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="328">
@@ -10525,7 +10518,7 @@
         <v>2.0</v>
       </c>
       <c r="I328" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="329">
@@ -10554,7 +10547,7 @@
         <v>2.0</v>
       </c>
       <c r="I329" s="1" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="330">
@@ -10583,7 +10576,7 @@
         <v>2.0</v>
       </c>
       <c r="I330" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="331">
@@ -10612,7 +10605,7 @@
         <v>3.0</v>
       </c>
       <c r="I331" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="332">
@@ -10625,9 +10618,7 @@
       <c r="C332" s="1">
         <v>85.0</v>
       </c>
-      <c r="D332" s="1" t="s">
-        <v>40</v>
-      </c>
+      <c r="D332" s="1"/>
       <c r="E332" s="1">
         <v>1835.0</v>
       </c>
@@ -10641,7 +10632,7 @@
         <v>2.0</v>
       </c>
       <c r="I332" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="333">
@@ -10670,7 +10661,7 @@
         <v>3.0</v>
       </c>
       <c r="I333" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="334">
@@ -10699,7 +10690,7 @@
         <v>2.0</v>
       </c>
       <c r="I334" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="335">
@@ -10728,7 +10719,7 @@
         <v>3.0</v>
       </c>
       <c r="I335" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="336">
@@ -10757,7 +10748,7 @@
         <v>3.0</v>
       </c>
       <c r="I336" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="337">
@@ -10786,7 +10777,7 @@
         <v>2.0</v>
       </c>
       <c r="I337" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="338">
@@ -10799,9 +10790,7 @@
       <c r="C338" s="1">
         <v>140.0</v>
       </c>
-      <c r="D338" s="1" t="s">
-        <v>40</v>
-      </c>
+      <c r="D338" s="1"/>
       <c r="E338" s="1">
         <v>2905.0</v>
       </c>
@@ -10815,7 +10804,7 @@
         <v>1.0</v>
       </c>
       <c r="I338" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="339">
@@ -10844,7 +10833,7 @@
         <v>3.0</v>
       </c>
       <c r="I339" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="340">
@@ -10873,7 +10862,7 @@
         <v>1.0</v>
       </c>
       <c r="I340" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="341">
@@ -10902,7 +10891,7 @@
         <v>1.0</v>
       </c>
       <c r="I341" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="342">
@@ -10931,7 +10920,7 @@
         <v>1.0</v>
       </c>
       <c r="I342" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="343">
@@ -10960,7 +10949,7 @@
         <v>1.0</v>
       </c>
       <c r="I343" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="344">
@@ -10989,7 +10978,7 @@
         <v>1.0</v>
       </c>
       <c r="I344" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="345">
@@ -11018,7 +11007,7 @@
         <v>3.0</v>
       </c>
       <c r="I345" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="346">
@@ -11047,7 +11036,7 @@
         <v>1.0</v>
       </c>
       <c r="I346" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="347">
@@ -11076,7 +11065,7 @@
         <v>3.0</v>
       </c>
       <c r="I347" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="348">
@@ -11105,7 +11094,7 @@
         <v>3.0</v>
       </c>
       <c r="I348" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="349">
@@ -11134,7 +11123,7 @@
         <v>3.0</v>
       </c>
       <c r="I349" s="1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="350">
@@ -11163,7 +11152,7 @@
         <v>3.0</v>
       </c>
       <c r="I350" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="351">
@@ -11192,7 +11181,7 @@
         <v>3.0</v>
       </c>
       <c r="I351" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="352">
@@ -11221,7 +11210,7 @@
         <v>1.0</v>
       </c>
       <c r="I352" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="353">
@@ -11250,7 +11239,7 @@
         <v>1.0</v>
       </c>
       <c r="I353" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="354">
@@ -11279,7 +11268,7 @@
         <v>1.0</v>
       </c>
       <c r="I354" s="1" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="355">
@@ -11308,7 +11297,7 @@
         <v>2.0</v>
       </c>
       <c r="I355" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="356">
@@ -11321,9 +11310,7 @@
       <c r="C356" s="1">
         <v>100.0</v>
       </c>
-      <c r="D356" s="1" t="s">
-        <v>40</v>
-      </c>
+      <c r="D356" s="1"/>
       <c r="E356" s="1">
         <v>2320.0</v>
       </c>
@@ -11337,7 +11324,7 @@
         <v>2.0</v>
       </c>
       <c r="I356" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="357">
@@ -11366,7 +11353,7 @@
         <v>3.0</v>
       </c>
       <c r="I357" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="358">
@@ -11395,7 +11382,7 @@
         <v>3.0</v>
       </c>
       <c r="I358" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="359">
@@ -11424,7 +11411,7 @@
         <v>3.0</v>
       </c>
       <c r="I359" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="360">
@@ -11453,7 +11440,7 @@
         <v>3.0</v>
       </c>
       <c r="I360" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="361">
@@ -11482,7 +11469,7 @@
         <v>2.0</v>
       </c>
       <c r="I361" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="362">
@@ -11511,7 +11498,7 @@
         <v>2.0</v>
       </c>
       <c r="I362" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="363">
@@ -11540,7 +11527,7 @@
         <v>3.0</v>
       </c>
       <c r="I363" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="364">
@@ -11569,7 +11556,7 @@
         <v>3.0</v>
       </c>
       <c r="I364" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="365">
@@ -11598,7 +11585,7 @@
         <v>1.0</v>
       </c>
       <c r="I365" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="366">
@@ -11627,7 +11614,7 @@
         <v>1.0</v>
       </c>
       <c r="I366" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="367">
@@ -11656,7 +11643,7 @@
         <v>1.0</v>
       </c>
       <c r="I367" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="368">
@@ -11685,7 +11672,7 @@
         <v>1.0</v>
       </c>
       <c r="I368" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="369">
@@ -11714,7 +11701,7 @@
         <v>1.0</v>
       </c>
       <c r="I369" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="370">
@@ -11743,7 +11730,7 @@
         <v>1.0</v>
       </c>
       <c r="I370" s="1" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="371">
@@ -11772,7 +11759,7 @@
         <v>1.0</v>
       </c>
       <c r="I371" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="372">
@@ -11801,7 +11788,7 @@
         <v>1.0</v>
       </c>
       <c r="I372" s="1" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="373">
@@ -11830,7 +11817,7 @@
         <v>1.0</v>
       </c>
       <c r="I373" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="374">
@@ -11859,7 +11846,7 @@
         <v>1.0</v>
       </c>
       <c r="I374" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="375">
@@ -11888,7 +11875,7 @@
         <v>1.0</v>
       </c>
       <c r="I375" s="1" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="376">
@@ -11901,9 +11888,7 @@
       <c r="C376" s="1">
         <v>151.0</v>
       </c>
-      <c r="D376" s="1" t="s">
-        <v>40</v>
-      </c>
+      <c r="D376" s="1"/>
       <c r="E376" s="1">
         <v>3035.0</v>
       </c>
@@ -11917,7 +11902,7 @@
         <v>1.0</v>
       </c>
       <c r="I376" s="1" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="377">
@@ -11946,7 +11931,7 @@
         <v>2.0</v>
       </c>
       <c r="I377" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="378">
@@ -11975,7 +11960,7 @@
         <v>3.0</v>
       </c>
       <c r="I378" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="379">
@@ -12004,7 +11989,7 @@
         <v>3.0</v>
       </c>
       <c r="I379" s="1" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="380">
@@ -12033,7 +12018,7 @@
         <v>1.0</v>
       </c>
       <c r="I380" s="1" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="381">
@@ -12062,7 +12047,7 @@
         <v>1.0</v>
       </c>
       <c r="I381" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="382">
@@ -12091,7 +12076,7 @@
         <v>3.0</v>
       </c>
       <c r="I382" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="383">
@@ -12120,7 +12105,7 @@
         <v>3.0</v>
       </c>
       <c r="I383" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="384">
@@ -12149,7 +12134,7 @@
         <v>3.0</v>
       </c>
       <c r="I384" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="385">
@@ -12178,7 +12163,7 @@
         <v>3.0</v>
       </c>
       <c r="I385" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="386">
@@ -12207,7 +12192,7 @@
         <v>3.0</v>
       </c>
       <c r="I386" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="387">
@@ -12236,7 +12221,7 @@
         <v>3.0</v>
       </c>
       <c r="I387" s="1" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="388">
@@ -12265,7 +12250,7 @@
         <v>1.0</v>
       </c>
       <c r="I388" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="389">
@@ -12294,7 +12279,7 @@
         <v>1.0</v>
       </c>
       <c r="I389" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="390">
@@ -12323,7 +12308,7 @@
         <v>1.0</v>
       </c>
       <c r="I390" s="1" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="391">
@@ -12352,7 +12337,7 @@
         <v>1.0</v>
       </c>
       <c r="I391" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="392">
@@ -12381,7 +12366,7 @@
         <v>3.0</v>
       </c>
       <c r="I392" s="1" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="393">
@@ -12410,7 +12395,7 @@
         <v>1.0</v>
       </c>
       <c r="I393" s="1" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="394">
@@ -12439,7 +12424,7 @@
         <v>1.0</v>
       </c>
       <c r="I394" s="1" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="395">
@@ -12468,7 +12453,7 @@
         <v>1.0</v>
       </c>
       <c r="I395" s="1" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="396">
@@ -12497,7 +12482,7 @@
         <v>2.0</v>
       </c>
       <c r="I396" s="1" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="397">
@@ -12526,7 +12511,7 @@
         <v>1.0</v>
       </c>
       <c r="I397" s="1" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="398">
@@ -12555,7 +12540,7 @@
         <v>1.0</v>
       </c>
       <c r="I398" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="399">
@@ -12584,7 +12569,7 @@
         <v>1.0</v>
       </c>
       <c r="I399" s="1" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
   </sheetData>

</xml_diff>